<commit_message>
updated BoM and description
</commit_message>
<xml_diff>
--- a/docs/hardware/ImportTest.xlsx
+++ b/docs/hardware/ImportTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHE\Documents\Git_Data\HelMoRo\docs\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6244D6-4D29-4390-B5F0-5A811BDD22CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E78374E-3999-41A0-806F-82596BF64395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D43A7108-50A9-4FCF-900B-676A8BDC7C7C}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" xr2:uid="{D43A7108-50A9-4FCF-900B-676A8BDC7C7C}"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
@@ -819,9 +819,6 @@
     <t>FIT 0186</t>
   </si>
   <si>
-    <t>HEL-06-01000-00</t>
-  </si>
-  <si>
     <t>HEL-06-01002-00</t>
   </si>
   <si>
@@ -1234,6 +1231,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>HEL-06-01000-01</t>
   </si>
 </sst>
 </file>
@@ -4520,8 +4520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C6E063-1877-40DA-BDBC-FD081DB60E9D}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4559,7 +4559,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4570,7 +4570,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>24</v>
@@ -4579,10 +4579,10 @@
         <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H2" s="2">
         <v>100</v>
@@ -4596,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>26</v>
@@ -4605,10 +4605,10 @@
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H3" s="2">
         <v>80</v>
@@ -4625,19 +4625,19 @@
         <v>27</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -4651,19 +4651,19 @@
         <v>28</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4677,16 +4677,16 @@
         <v>29</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H6" s="2">
         <v>30</v>
@@ -4700,19 +4700,19 @@
         <v>4</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>31</v>
+        <v>169</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H7" s="2">
         <v>3</v>
@@ -4726,19 +4726,19 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H8" s="2">
         <v>4</v>
@@ -4752,22 +4752,22 @@
         <v>4</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -4778,19 +4778,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H10" s="2">
         <v>71.3</v>
@@ -4804,22 +4804,22 @@
         <v>1</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -4830,22 +4830,22 @@
         <v>1</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4856,17 +4856,17 @@
         <v>2</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H13" s="2">
         <v>70</v>
@@ -4880,22 +4880,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -4906,19 +4906,19 @@
         <v>1</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H15" s="2">
         <v>39</v>
@@ -4932,19 +4932,19 @@
         <v>1</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H16" s="2">
         <v>113</v>
@@ -4958,19 +4958,19 @@
         <v>1</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H17" s="2">
         <v>15</v>
@@ -4984,19 +4984,19 @@
         <v>1</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -5008,19 +5008,19 @@
         <v>1</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -5032,19 +5032,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H20" s="2">
         <v>320</v>
@@ -5058,22 +5058,22 @@
         <v>1</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -5084,19 +5084,19 @@
         <v>1</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H22" s="2">
         <v>200</v>
@@ -5110,22 +5110,22 @@
         <v>6</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5136,22 +5136,22 @@
         <v>4</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -5162,19 +5162,19 @@
         <v>16</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H25" s="2">
         <v>3</v>
@@ -5188,19 +5188,19 @@
         <v>1</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H26" s="2">
         <v>38</v>
@@ -5214,22 +5214,22 @@
         <v>1</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5240,19 +5240,19 @@
         <v>1</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H28" s="2">
         <v>100</v>
@@ -5266,19 +5266,19 @@
         <v>1</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H29" s="2">
         <v>50</v>
@@ -5292,19 +5292,19 @@
         <v>1</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H30" s="2">
         <v>50</v>
@@ -5318,19 +5318,19 @@
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="G31" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H31" s="2">
         <v>11.3</v>
@@ -5344,19 +5344,19 @@
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="E32" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="G32" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H32" s="2">
         <v>6</v>
@@ -5370,22 +5370,22 @@
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5396,22 +5396,22 @@
         <v>1</v>
       </c>
       <c r="C34" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G34" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5422,22 +5422,22 @@
         <v>1</v>
       </c>
       <c r="C35" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="G35" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -5448,22 +5448,22 @@
         <v>1</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5474,22 +5474,22 @@
         <v>1</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5500,22 +5500,22 @@
         <v>2</v>
       </c>
       <c r="C38" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="H38" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5526,22 +5526,22 @@
         <v>1</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5552,22 +5552,22 @@
         <v>4</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5578,22 +5578,22 @@
         <v>4</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5604,22 +5604,22 @@
         <v>2</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5630,22 +5630,22 @@
         <v>4</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5656,22 +5656,22 @@
         <v>4</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5682,22 +5682,22 @@
         <v>1</v>
       </c>
       <c r="C45" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="17" t="s">
-        <v>93</v>
-      </c>
       <c r="E45" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5708,22 +5708,22 @@
         <v>1</v>
       </c>
       <c r="C46" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D46" s="17" t="s">
-        <v>95</v>
-      </c>
       <c r="E46" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5734,22 +5734,22 @@
         <v>2</v>
       </c>
       <c r="C47" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>97</v>
-      </c>
       <c r="G47" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5760,22 +5760,22 @@
         <v>5</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -5786,22 +5786,22 @@
         <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5812,22 +5812,22 @@
         <v>4</v>
       </c>
       <c r="C50" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D50" s="17" t="s">
-        <v>144</v>
-      </c>
       <c r="E50" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7282,7 +7282,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C17A5DE6-F76F-4374-ABFC-06AD0B1D1265}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F74BA4D6-0AA6-4B4C-B855-94335047CF04}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="HelblingDocs"/>

</xml_diff>